<commit_message>
weerstanden voor de rgb leds toegevoegd
</commit_message>
<xml_diff>
--- a/ISA Ouderen/Deurbel ontvanger/BOM.xlsx
+++ b/ISA Ouderen/Deurbel ontvanger/BOM.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arne\GIT\GITHUB\IsaLib\ISA Ouderen\Deurbel ontvanger\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15855" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>PCA9635PW</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
   <si>
     <t>Verzendkosten</t>
   </si>
@@ -43,6 +45,231 @@
   </si>
   <si>
     <t>Product</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>0.1µ</t>
+  </si>
+  <si>
+    <t>C-EU025-024X044</t>
+  </si>
+  <si>
+    <t>CAPACITOR, European symbol</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>22pf</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>10µ</t>
+  </si>
+  <si>
+    <t>CPOL-EUE1.8-4</t>
+  </si>
+  <si>
+    <t>POLARIZED CAPACITOR, European symbol</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>DIODE-D-5</t>
+  </si>
+  <si>
+    <t>DIODE</t>
+  </si>
+  <si>
+    <t>FTDI</t>
+  </si>
+  <si>
+    <t>MA06-1</t>
+  </si>
+  <si>
+    <t>PIN HEADER</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>MEGA8-P</t>
+  </si>
+  <si>
+    <t>MICROCONTROLLER</t>
+  </si>
+  <si>
+    <t>IC2</t>
+  </si>
+  <si>
+    <t>MCP1702-33</t>
+  </si>
+  <si>
+    <t>MCP1702Z</t>
+  </si>
+  <si>
+    <t>200 mA, Low Power Low Dropout Voltage Regulator</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>BATT</t>
+  </si>
+  <si>
+    <t>M02LOCK_LONGPADS</t>
+  </si>
+  <si>
+    <t>Header 2</t>
+  </si>
+  <si>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>PINHD-1X4/90</t>
+  </si>
+  <si>
+    <t>JP4</t>
+  </si>
+  <si>
+    <t>JP5</t>
+  </si>
+  <si>
+    <t>JP6</t>
+  </si>
+  <si>
+    <t>AVR-ISP-6VERT</t>
+  </si>
+  <si>
+    <t>AVR ISP-6 Serial Programming Header</t>
+  </si>
+  <si>
+    <t>JP7</t>
+  </si>
+  <si>
+    <t>PINHD-2X8</t>
+  </si>
+  <si>
+    <t>JP10</t>
+  </si>
+  <si>
+    <t>M02PTH3</t>
+  </si>
+  <si>
+    <t>Standard 2-pin 0.1 header. Use with"</t>
+  </si>
+  <si>
+    <t>JP11</t>
+  </si>
+  <si>
+    <t>M08LONGPADS</t>
+  </si>
+  <si>
+    <t>Header 8</t>
+  </si>
+  <si>
+    <t>JP13</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED-TRICOLOR-5050NO_IC</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>LED3</t>
+  </si>
+  <si>
+    <t>LED4</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>BC547</t>
+  </si>
+  <si>
+    <t>NPN Transistor</t>
+  </si>
+  <si>
+    <t>Q15</t>
+  </si>
+  <si>
+    <t>XTAL/S</t>
+  </si>
+  <si>
+    <t>CRYSTAL</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>R-EU_0207/2V</t>
+  </si>
+  <si>
+    <t>RESISTOR, European symbol</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>R-EU_0207/7</t>
+  </si>
+  <si>
+    <t>U$1</t>
+  </si>
+  <si>
+    <t>PCA9635</t>
+  </si>
+  <si>
+    <t>16 pin PWM with 8 bit per-channel PWM, and 7 bit group PWM on I2C bus</t>
+  </si>
+  <si>
+    <t>U$3</t>
+  </si>
+  <si>
+    <t>RFM12B</t>
+  </si>
+  <si>
+    <t>16mhz</t>
+  </si>
+  <si>
+    <t>Batterijhouder (4xAA)</t>
+  </si>
+  <si>
+    <t>Witte leds</t>
   </si>
 </sst>
 </file>
@@ -52,7 +279,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -72,6 +299,14 @@
       <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -101,18 +336,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -438,23 +683,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:F10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.75" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
+    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="5" max="5" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28">
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -462,184 +708,516 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="6">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="1"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="1"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="1"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>62</v>
+      </c>
+      <c r="C37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="F41" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="G41" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H41" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="I41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="E10" s="1">
-        <v>8.1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="2:5">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:5">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:5">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="2:5">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="2:5">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="2:5">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="2:5">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="2:5">
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="2:5">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="2:5">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="2:5">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="2:5">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="2:5">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
PCB afgemaakt, BOM lijst aangevuld.
</commit_message>
<xml_diff>
--- a/ISA Ouderen/Deurbel ontvanger/BOM.xlsx
+++ b/ISA Ouderen/Deurbel ontvanger/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="87">
   <si>
     <t>Verzendkosten</t>
   </si>
@@ -50,9 +50,6 @@
     <t>C1</t>
   </si>
   <si>
-    <t>0.1µ</t>
-  </si>
-  <si>
     <t>C-EU025-024X044</t>
   </si>
   <si>
@@ -263,21 +260,41 @@
     <t>RFM12B</t>
   </si>
   <si>
-    <t>16mhz</t>
-  </si>
-  <si>
-    <t>Batterijhouder (4xAA)</t>
-  </si>
-  <si>
     <t>Witte leds</t>
+  </si>
+  <si>
+    <t>Boxed Header 10p Haaks</t>
+  </si>
+  <si>
+    <t>Boxed Header 16p Haaks</t>
+  </si>
+  <si>
+    <t>Boxed header snoer 10p</t>
+  </si>
+  <si>
+    <t>Boxed header snoer 16p</t>
+  </si>
+  <si>
+    <t>Kristal 16 MHz mini</t>
+  </si>
+  <si>
+    <t>Atmega328P-PU</t>
+  </si>
+  <si>
+    <t>Spoel 33mH 30mA</t>
+  </si>
+  <si>
+    <t>Batterijhouder 2x AA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00_-"/>
+    <numFmt numFmtId="169" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -336,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -344,6 +361,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -683,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -694,7 +714,7 @@
     <col min="1" max="1" width="8.75" customWidth="1"/>
     <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="17.375" customWidth="1"/>
-    <col min="4" max="4" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="31.125" customWidth="1"/>
     <col min="5" max="5" width="16.375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -730,10 +750,12 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E6" s="1"/>
+      <c r="B6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="F6" s="6">
         <v>1</v>
       </c>
@@ -741,10 +763,12 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="1"/>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.55000000000000004</v>
+      </c>
       <c r="F7" s="6">
         <v>4</v>
       </c>
@@ -778,441 +802,486 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>9</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
       <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
         <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>9</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
       <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
         <v>9</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
         <v>8</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>9</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
         <v>9</v>
-      </c>
-      <c r="D19" t="s">
-        <v>10</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>24</v>
-      </c>
-      <c r="D20" t="s">
-        <v>25</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>27</v>
-      </c>
-      <c r="D21" t="s">
-        <v>28</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="6"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>30</v>
       </c>
-      <c r="C22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1">
+        <v>3.35</v>
+      </c>
       <c r="F22" s="6"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>33</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>34</v>
       </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1">
+        <v>0.95</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>37</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>38</v>
-      </c>
-      <c r="D24" t="s">
-        <v>39</v>
       </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.6</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
         <v>41</v>
       </c>
-      <c r="D26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="1"/>
+      <c r="B26" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="1"/>
+      <c r="B27" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>44</v>
-      </c>
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="1"/>
+      <c r="B28" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
-      </c>
-      <c r="B33" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>57</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="8"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C34" t="s">
-        <v>57</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" s="8"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="E35" s="8">
+        <v>0.5</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="E36" s="8">
+        <v>0.5</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" t="s">
-        <v>63</v>
+        <v>56</v>
+      </c>
+      <c r="E37" s="8">
+        <v>0.5</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D38" t="s">
-        <v>66</v>
+        <v>56</v>
+      </c>
+      <c r="E38" s="8">
+        <v>0.5</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="D39" t="s">
-        <v>70</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="E39" s="8"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" t="s">
-        <v>72</v>
+        <v>63</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D40" t="s">
-        <v>70</v>
+        <v>65</v>
+      </c>
+      <c r="E40" s="8">
+        <v>0.4</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D41" t="s">
-        <v>76</v>
-      </c>
-      <c r="E41" s="1">
-        <v>2.8</v>
-      </c>
-      <c r="F41" s="1">
-        <v>2</v>
-      </c>
-      <c r="G41" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="H41" s="1">
-        <v>8.1</v>
-      </c>
-      <c r="I41" t="s">
-        <v>4</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E41" s="8"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H43" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="I43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" t="s">
         <v>77</v>
       </c>
-      <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" t="s">
-        <v>78</v>
+      <c r="C44" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E45" s="9">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Een print met daarop 5mm rgb leds ipv 4 losse printjes met smd leds. Dit ivm de ruimte in de lamp voor de batterijen. Kostprijs is ook lager :P
</commit_message>
<xml_diff>
--- a/ISA Ouderen/Deurbel ontvanger/BOM.xlsx
+++ b/ISA Ouderen/Deurbel ontvanger/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="91">
   <si>
     <t>Verzendkosten</t>
   </si>
@@ -285,6 +285,18 @@
   </si>
   <si>
     <t>Okaphone</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>NEE</t>
+  </si>
+  <si>
+    <t>al binnen</t>
+  </si>
+  <si>
+    <t>270 en 330</t>
   </si>
 </sst>
 </file>
@@ -833,654 +845,720 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.875" customWidth="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1"/>
-    <col min="3" max="3" width="17.375" customWidth="1"/>
-    <col min="4" max="4" width="18.75" customWidth="1"/>
-    <col min="5" max="5" width="25.25" customWidth="1"/>
-    <col min="6" max="6" width="43.875" customWidth="1"/>
-    <col min="7" max="7" width="11.875" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
+    <col min="2" max="2" width="2.875" customWidth="1"/>
+    <col min="3" max="3" width="24.375" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="5" max="5" width="18.75" customWidth="1"/>
+    <col min="6" max="6" width="25.25" customWidth="1"/>
+    <col min="7" max="7" width="43.875" customWidth="1"/>
+    <col min="8" max="8" width="11.875" customWidth="1"/>
+    <col min="9" max="9" width="13.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="16"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="16"/>
-      <c r="G5" s="4" t="s">
-        <v>1</v>
-      </c>
+      <c r="G5" s="16"/>
       <c r="H5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="6">
         <v>3</v>
       </c>
-      <c r="I6" s="6">
-        <f>(A6*G6)+H6</f>
+      <c r="J6" s="6">
+        <f>(B6*H6)+I6</f>
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="10">
         <v>4</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="11">
+      <c r="G7" s="10"/>
+      <c r="H7" s="11">
         <v>0.45</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12">
-        <f t="shared" ref="I7:I33" si="0">(A7*G7)+H7</f>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12">
+        <f t="shared" ref="J7:J33" si="0">(B7*H7)+I7</f>
         <v>1.8</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>52</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>0.6</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6">
+      <c r="I8" s="6"/>
+      <c r="J8" s="6">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>55</v>
       </c>
       <c r="E9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="11">
+      <c r="H9" s="11">
         <v>0.75</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12">
+      <c r="I9" s="12"/>
+      <c r="J9" s="12">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" s="5" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>0.25</v>
       </c>
-      <c r="H10" s="6"/>
-      <c r="I10" s="14">
+      <c r="I10" s="6"/>
+      <c r="J10" s="14">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
-        <v>1</v>
-      </c>
-      <c r="B11" s="13" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="10">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="11">
+      <c r="G11" s="10"/>
+      <c r="H11" s="11">
         <v>0.35</v>
       </c>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12">
+      <c r="I11" s="12"/>
+      <c r="J11" s="12">
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" s="5" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>0.85</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="14">
+      <c r="I12" s="6"/>
+      <c r="J12" s="14">
         <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="10">
         <v>8</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="C13" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="G13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="11">
+      <c r="H13" s="11">
         <v>0.02</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12">
-        <f t="shared" ref="I13" si="1">(A13*G13)+H13</f>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12">
+        <f t="shared" ref="J13" si="1">(B13*H13)+I13</f>
         <v>0.16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="10">
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="G14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="11">
+      <c r="H14" s="11">
         <v>0.02</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12">
+      <c r="I14" s="12"/>
+      <c r="J14" s="12">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>60</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>5</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>59</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>80</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>0.06</v>
       </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6">
+      <c r="I15" s="6"/>
+      <c r="J15" s="6">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="10">
         <v>2</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="C16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="F16" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="G16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="11">
+      <c r="H16" s="11">
         <v>0.08</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12">
+      <c r="I16" s="12"/>
+      <c r="J16" s="12">
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>63</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>64</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>65</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>0.08</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6">
+      <c r="I17" s="6"/>
+      <c r="J17" s="6">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>1</v>
-      </c>
-      <c r="B18" s="10" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="10">
+        <v>1</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F18" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="G18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="11">
+      <c r="H18" s="11">
         <v>0.1</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12">
+      <c r="I18" s="12"/>
+      <c r="J18" s="12">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>30</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>67</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>29</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>0.4</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6">
+      <c r="I19" s="6"/>
+      <c r="J19" s="6">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
-        <v>1</v>
-      </c>
-      <c r="B20" s="10" t="s">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="10">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="E20" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="F20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="G20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="11">
+      <c r="H20" s="11">
         <v>0.08</v>
       </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12">
+      <c r="I20" s="12"/>
+      <c r="J20" s="12">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21">
         <v>2</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>7</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>5</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>59</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>68</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>0.12</v>
       </c>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6">
+      <c r="I21" s="6"/>
+      <c r="J21" s="6">
         <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>1</v>
-      </c>
-      <c r="B22" s="13" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="E22" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F22" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="G22" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G22" s="11">
+      <c r="H22" s="11">
         <v>0.35</v>
       </c>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12">
+      <c r="I22" s="12"/>
+      <c r="J22" s="12">
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
       </c>
       <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
         <v>73</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>22</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>0.65</v>
       </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6">
+      <c r="I23" s="6"/>
+      <c r="J23" s="6">
         <f t="shared" si="0"/>
         <v>0.65</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>1</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>84</v>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="10">
+        <v>1</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>84</v>
       </c>
       <c r="D24" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="F24" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="G24" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="11">
+      <c r="H24" s="11">
         <v>0.1</v>
       </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12">
+      <c r="I24" s="12"/>
+      <c r="J24" s="12">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>12</v>
-      </c>
-      <c r="C25" t="s">
-        <v>13</v>
       </c>
       <c r="D25" t="s">
         <v>13</v>
       </c>
       <c r="E25" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
         <v>12</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>0.2</v>
       </c>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6">
+      <c r="I25" s="6"/>
+      <c r="J25" s="6">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="10">
         <v>4</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="C26" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="E26" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="F26" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="11">
+      <c r="G26" s="10"/>
+      <c r="H26" s="11">
         <v>0.5</v>
       </c>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12">
+      <c r="I26" s="12"/>
+      <c r="J26" s="12">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>1</v>
-      </c>
-      <c r="B27" s="10" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="10">
+        <v>1</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="E27" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="F27" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="G27" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G27" s="11">
+      <c r="H27" s="11">
         <v>0.95</v>
       </c>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12">
+      <c r="I27" s="12"/>
+      <c r="J27" s="12">
         <f t="shared" si="0"/>
         <v>0.95</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" s="5" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>16</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>77</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>15</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>17</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>3.35</v>
       </c>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6">
+      <c r="I28" s="6"/>
+      <c r="J28" s="6">
         <f t="shared" si="0"/>
         <v>3.35</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
-        <v>1</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>38</v>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B29" s="10">
+        <v>1</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>38</v>
@@ -1489,31 +1567,31 @@
         <v>38</v>
       </c>
       <c r="E29" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="G29" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G29" s="11">
+      <c r="H29" s="11">
         <v>2.8</v>
       </c>
-      <c r="H29" s="12">
+      <c r="I29" s="12">
         <v>2.5</v>
       </c>
-      <c r="I29" s="12">
+      <c r="J29" s="12">
         <f t="shared" si="0"/>
         <v>5.3</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>1</v>
       </c>
       <c r="C30" t="s">
         <v>40</v>
@@ -1522,64 +1600,67 @@
         <v>40</v>
       </c>
       <c r="E30" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>6</v>
       </c>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6">
+      <c r="I30" s="6"/>
+      <c r="J30" s="6">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
-        <v>1</v>
-      </c>
-      <c r="B31" s="10" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B31" s="10">
+        <v>1</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="G31" s="11">
+      <c r="H31" s="11">
         <v>3</v>
       </c>
-      <c r="I31" s="6">
+      <c r="J31" s="6">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I32" s="6">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J32" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I33" s="6">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J33" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="7"/>
+    <row r="34" spans="2:10" ht="21" x14ac:dyDescent="0.35">
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
-      <c r="G34" s="8">
-        <f>SUM(G6:G33)</f>
+      <c r="G34" s="7"/>
+      <c r="H34" s="8">
+        <f>SUM(H6:H33)</f>
         <v>22.66</v>
       </c>
-      <c r="H34" s="9">
-        <f>SUM(H29:H33)</f>
+      <c r="I34" s="9">
+        <f>SUM(I29:I33)</f>
         <v>2.5</v>
       </c>
-      <c r="I34" s="9">
-        <f>SUM(I6:I33)</f>
+      <c r="J34" s="9">
+        <f>SUM(J6:J33)</f>
         <v>32.200000000000003</v>
       </c>
     </row>

</xml_diff>